<commit_message>
file names, st task xlsx bug
</commit_message>
<xml_diff>
--- a/backend/data/checkExcel.xlsx
+++ b/backend/data/checkExcel.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
   <si>
     <t>Дата завдання</t>
   </si>
@@ -58,40 +58,46 @@
     <t>Коментар</t>
   </si>
   <si>
-    <t>15-01-2019</t>
+    <t>18-01-2019</t>
+  </si>
+  <si>
+    <t>ЛУЦЬКВОДОКАНАЛ</t>
+  </si>
+  <si>
+    <t>Тестовий</t>
+  </si>
+  <si>
+    <t>Тестова</t>
+  </si>
+  <si>
+    <t>Т3</t>
+  </si>
+  <si>
+    <t>Т33</t>
+  </si>
+  <si>
+    <t>Т1</t>
+  </si>
+  <si>
+    <t>Т55</t>
   </si>
   <si>
     <t/>
   </si>
   <si>
-    <t>Шевченківський</t>
-  </si>
-  <si>
-    <t>Львівська</t>
-  </si>
-  <si>
-    <t>3</t>
-  </si>
-  <si>
-    <t>Павлова Павла Павловича</t>
-  </si>
-  <si>
-    <t>505050555</t>
-  </si>
-  <si>
-    <t>2019-01-25T22:00:00.000Z</t>
-  </si>
-  <si>
-    <t>15012019003</t>
-  </si>
-  <si>
-    <t>Коментарик</t>
-  </si>
-  <si>
-    <t>15012019002</t>
-  </si>
-  <si>
-    <t>15012019001</t>
+    <t>Тестовий Тест Тестович</t>
+  </si>
+  <si>
+    <t>+38097334523</t>
+  </si>
+  <si>
+    <t>09-02-2019</t>
+  </si>
+  <si>
+    <t>18012019001</t>
+  </si>
+  <si>
+    <t>Тестовий коментар</t>
   </si>
 </sst>
 </file>
@@ -154,7 +160,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O4"/>
+  <dimension ref="A1:O2"/>
   <sheetViews>
     <sheetView showGridLines="1" workbookViewId="0" rightToLeft="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100"/>
   </sheetViews>
@@ -241,128 +247,34 @@
         <v>19</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="H2" s="0" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="I2" s="0" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="J2" s="0" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="K2" s="0" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="L2" s="0" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="M2" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="N2" s="0" t="s">
         <v>23</v>
       </c>
-      <c r="N2" s="0" t="s">
-        <v>16</v>
-      </c>
       <c r="O2" s="0" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15">
-      <c r="A3" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="B3" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="C3" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="D3" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="E3" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="F3" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="G3" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="H3" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="I3" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="J3" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="K3" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="L3" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="M3" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="N3" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="O3" s="0" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15">
-      <c r="A4" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="B4" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="C4" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="D4" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="E4" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="F4" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="G4" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="H4" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="I4" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="J4" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="K4" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="L4" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="M4" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="N4" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="O4" s="0" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>